<commit_message>
erste drei Kapitel auf Quellen und Reschtschreibung geprueft. Bei Minijobs die AN-Rentenpauschalenfrage implementiert.
</commit_message>
<xml_diff>
--- a/src/main/2 insert Sozialversicherungsdaten/9 Minijobbeitraege.xlsx
+++ b/src/main/2 insert Sozialversicherungsdaten/9 Minijobbeitraege.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\2 insert Sozialversicherungsdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076D00ED-603A-4B83-83C0-D95FB23797CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4DB338-5D54-47AC-B18A-FD76D0DCB864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2292" yWindow="1752" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Daten</t>
   </si>
@@ -49,12 +49,6 @@
     <t>nein</t>
   </si>
   <si>
-    <t>Arbeitgeberbeitrag Rentenversicherung in Prozent</t>
-  </si>
-  <si>
-    <t>Arbeitnehmerbeitrag Rentenversicherung in Prozent</t>
-  </si>
-  <si>
     <t>U1-Umlage in Prozent</t>
   </si>
   <si>
@@ -67,10 +61,19 @@
     <t>Pauschalsteuer in Prozent</t>
   </si>
   <si>
-    <t>Krankenversicherung in Prozent</t>
-  </si>
-  <si>
     <t>01.01.2024</t>
+  </si>
+  <si>
+    <t>Zahlt Arbeitnehmer Rentenpauschale?</t>
+  </si>
+  <si>
+    <t>Arbeitgeberpauschale Krankenversicherung in Prozent</t>
+  </si>
+  <si>
+    <t>Arbeitgeberpauschale Rentenversicherung in Prozent</t>
+  </si>
+  <si>
+    <t>Arbeitnehmerpauschale Rentenversicherung in Prozent</t>
   </si>
 </sst>
 </file>
@@ -399,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,66 +432,74 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2">
-        <v>3.6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2">
-        <v>1.1000000000000001</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>0.24</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>0.06</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -501,7 +512,7 @@
           <x14:formula1>
             <xm:f>Tabelle2!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
+          <xm:sqref>B2:B3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>